<commit_message>
medel.sol och medel.regn i EN tabell
</commit_message>
<xml_diff>
--- a/väder (1).xlsx
+++ b/väder (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dick\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dick\Documents\BI-relaterade programspråk\Restauran inlupp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5378AB71-2889-4DF8-9DD6-CD53CC08C43F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AAAEF4-AC20-4E54-858E-EAC9660957D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{438B0215-085D-4CFB-846C-591540B41AA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{438B0215-085D-4CFB-846C-591540B41AA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Stad</t>
   </si>
@@ -102,50 +102,14 @@
     <t>Sol(tim/dag)</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Nederbörd(mm/dag)</t>
-  </si>
-  <si>
-    <t>Hoburg A</t>
-  </si>
-  <si>
-    <t>Svenska Högarna A</t>
-  </si>
-  <si>
-    <t>Visby Flygplats</t>
-  </si>
-  <si>
-    <t>Nordkoster A</t>
-  </si>
-  <si>
-    <t>Ölands Norra Udde A</t>
-  </si>
-  <si>
-    <t>Stockholm A</t>
-  </si>
-  <si>
-    <t>Luleå Flygplats</t>
-  </si>
-  <si>
-    <t>Karlstad A</t>
-  </si>
-  <si>
-    <t>Tarfala</t>
-  </si>
-  <si>
-    <t>NEDERBÖRD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +132,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +161,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -286,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -296,62 +279,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
-      <border outline="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -392,33 +362,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D1C865A-1ABC-49D5-A1E1-55F16608B3CB}" name="Tabell1" displayName="Tabell1" ref="A1:D20" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:D20" xr:uid="{BA2E7642-A008-4B1C-973C-D3B0BD36D2CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D1C865A-1ABC-49D5-A1E1-55F16608B3CB}" name="Tabell1" displayName="Tabell1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:E20" xr:uid="{BA2E7642-A008-4B1C-973C-D3B0BD36D2CD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
     <sortCondition descending="1" ref="B1:B20"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A2A3C49C-F89A-4F05-9C37-346ACF09E31E}" name="Stad"/>
     <tableColumn id="2" xr3:uid="{45A4A085-39C1-4FA3-9693-FB297C9C60FA}" name="Sol(sek/dag)"/>
-    <tableColumn id="3" xr3:uid="{256C51D2-9C19-4B4A-8ED0-E766BE54360C}" name="Sol(Min/dag)" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{256C51D2-9C19-4B4A-8ED0-E766BE54360C}" name="Sol(Min/dag)" dataDxfId="2">
       <calculatedColumnFormula>SUM(B2/60)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9A474081-2A69-40D5-926B-73C2EE67F3E6}" name="Sol(tim/dag)" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{9A474081-2A69-40D5-926B-73C2EE67F3E6}" name="Sol(tim/dag)" dataDxfId="1">
       <calculatedColumnFormula>SUM(C2/60)</calculatedColumnFormula>
     </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6592CC97-BA6B-4A67-89C6-4C87C4EEF77D}" name="Table1" displayName="Table1" ref="A26:D45" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="A26:D45" xr:uid="{25B41349-FFDA-4097-BD84-51829A7B2574}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A8E03235-2CEC-4C50-8A08-D706E9AA60FD}" name="Stad"/>
-    <tableColumn id="2" xr3:uid="{5B6EF135-F615-45CD-A770-C96FFA9412A6}" name="Column1"/>
-    <tableColumn id="3" xr3:uid="{51526AF9-9F73-479D-B58F-118932DE1DB1}" name="Column2"/>
-    <tableColumn id="4" xr3:uid="{9F3B995C-52D1-4C3E-889F-F2B7C128D17D}" name="Nederbörd(mm/dag)"/>
+    <tableColumn id="5" xr3:uid="{40B187CE-0344-4652-ADF8-8FC210D3F489}" name="Nederbörd(mm/dag)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -721,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB34484-1CB8-470C-93C7-75388BEEFF85}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,10 +690,10 @@
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -748,8 +706,11 @@
       <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -764,8 +725,11 @@
         <f t="shared" si="0"/>
         <v>0.25817850947740245</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5.4207416968673081E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -780,8 +744,11 @@
         <f t="shared" si="0"/>
         <v>0.25101964769647694</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4.2919998307736656E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -796,8 +763,11 @@
         <f t="shared" si="0"/>
         <v>0.24733061750069085</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>7.1644343117697074E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -812,8 +782,11 @@
         <f t="shared" si="0"/>
         <v>0.24514436424021971</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>6.1829119278125982E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -828,8 +801,11 @@
         <f t="shared" si="0"/>
         <v>0.24100714546134319</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>7.7132926129657678E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -844,8 +820,11 @@
         <f t="shared" si="0"/>
         <v>0.24004517624895846</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4.9250306149883218E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -860,8 +839,11 @@
         <f t="shared" si="0"/>
         <v>0.22365502423233316</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4.711111111111109E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -876,8 +858,11 @@
         <f t="shared" si="0"/>
         <v>0.22149955703712992</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>8.7810887988208325E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -892,8 +877,11 @@
         <f t="shared" si="0"/>
         <v>0.22106265805588649</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>7.3356678288180904E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -908,8 +896,11 @@
         <f t="shared" si="0"/>
         <v>0.2180168150518593</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>6.1870142546693659E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -924,8 +915,11 @@
         <f t="shared" si="0"/>
         <v>0.2166520715335688</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>6.4138507320153429E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -940,8 +934,11 @@
         <f t="shared" si="0"/>
         <v>0.20915258532405373</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="15">
+        <v>9.2682755011678858E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -956,8 +953,11 @@
         <f t="shared" si="0"/>
         <v>0.20812534107560443</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="8">
+        <v>7.4267784537472112E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -972,8 +972,11 @@
         <f t="shared" si="0"/>
         <v>0.20182878352990899</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="15">
+        <v>0.1025376701871161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -988,8 +991,11 @@
         <f t="shared" si="0"/>
         <v>0.19391482805145102</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="8">
+        <v>6.366420638055327E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1004,8 +1010,11 @@
         <f t="shared" si="0"/>
         <v>0.18882360556681829</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="15">
+        <v>7.5702172099005094E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1020,8 +1029,11 @@
         <f t="shared" si="0"/>
         <v>0.17659743557589816</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="8">
+        <v>5.5961427114778001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1036,8 +1048,11 @@
         <f t="shared" si="0"/>
         <v>0.16912905277912557</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="15">
+        <v>9.3925004516251742E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1052,198 +1067,69 @@
         <f t="shared" si="0"/>
         <v>0.12312031691581141</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27">
-        <v>5.4207416968673081E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28">
-        <v>4.2919998307736656E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29">
-        <v>7.1644343117697074E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30">
-        <v>6.1829119278125982E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31">
-        <v>7.7132926129657678E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32">
-        <v>4.9250306149883218E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33">
-        <v>4.711111111111109E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34">
-        <v>8.7810887988208325E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35">
-        <v>7.3356678288180904E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36">
-        <v>6.1870142546693659E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37">
-        <v>6.4138507320153429E-2</v>
-      </c>
+      <c r="E20" s="7">
+        <v>0.11243186028049763</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="10">
-        <v>9.2682755011678858E-2</v>
-      </c>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="11">
-        <v>7.4267784537472112E-2</v>
-      </c>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="10">
-        <v>0.1025376701871161</v>
-      </c>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="11">
-        <v>6.366420638055327E-2</v>
-      </c>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="10">
-        <v>7.5702172099005094E-2</v>
-      </c>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="11">
-        <v>5.5961427114778001E-2</v>
-      </c>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="10">
-        <v>9.3925004516251742E-2</v>
-      </c>
+      <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="10">
-        <v>0.11243186028049763</v>
-      </c>
+      <c r="A45" s="9"/>
+      <c r="D45" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>